<commit_message>
the mountain is liquid
</commit_message>
<xml_diff>
--- a/earlyUserStudy/earlyStudyResults.xlsx
+++ b/earlyUserStudy/earlyStudyResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28760" yWindow="-1080" windowWidth="19920" windowHeight="18960" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="29220" yWindow="560" windowWidth="24800" windowHeight="17320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="earlySanalysis" sheetId="3" r:id="rId1"/>
@@ -31,6 +31,46 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+  <si>
+    <t>Resizing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimizing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hiding</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exiting</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action Tabs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Action Bar</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -117,10 +157,6 @@
   </si>
   <si>
     <t>Hiding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exiting</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -363,42 +399,6 @@
     <t>Avg</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
-  <si>
-    <t>Resizing</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Minimizing</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hiding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exiting</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Action Tabs</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
@@ -1497,6 +1497,15 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1533,6 +1542,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1549,51 +1594,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1739,11 +1739,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="552354632"/>
-        <c:axId val="552341736"/>
+        <c:axId val="541572824"/>
+        <c:axId val="541372984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="552354632"/>
+        <c:axId val="541572824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,13 +1786,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="552341736"/>
+        <c:crossAx val="541372984"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="552341736"/>
+        <c:axId val="541372984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,7 +1816,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="552354632"/>
+        <c:crossAx val="541572824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1955,11 +1955,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="550823128"/>
-        <c:axId val="550816152"/>
+        <c:axId val="541152312"/>
+        <c:axId val="541145336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="550823128"/>
+        <c:axId val="541152312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2002,13 +2002,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="550816152"/>
+        <c:crossAx val="541145336"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="550816152"/>
+        <c:axId val="541145336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2032,7 +2032,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550823128"/>
+        <c:crossAx val="541152312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2171,11 +2171,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="550781960"/>
-        <c:axId val="550774984"/>
+        <c:axId val="541111176"/>
+        <c:axId val="541104200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="550781960"/>
+        <c:axId val="541111176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2218,13 +2218,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="550774984"/>
+        <c:crossAx val="541104200"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="550774984"/>
+        <c:axId val="541104200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2248,7 +2248,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550781960"/>
+        <c:crossAx val="541111176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2387,11 +2387,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="550740120"/>
-        <c:axId val="550733144"/>
+        <c:axId val="541069336"/>
+        <c:axId val="526691256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="550740120"/>
+        <c:axId val="541069336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2434,13 +2434,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="550733144"/>
+        <c:crossAx val="526691256"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="550733144"/>
+        <c:axId val="526691256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2464,7 +2464,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550740120"/>
+        <c:crossAx val="541069336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2515,10 +2515,10 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.611111111111111</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.222222222222222</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.888888888888889</c:v>
@@ -2537,11 +2537,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="550665160"/>
-        <c:axId val="550675304"/>
+        <c:axId val="526731032"/>
+        <c:axId val="526728872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="550665160"/>
+        <c:axId val="526731032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2565,13 +2565,13 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550675304"/>
+        <c:crossAx val="526728872"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="550675304"/>
+        <c:axId val="526728872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,7 +2596,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550665160"/>
+        <c:crossAx val="526731032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -2643,10 +2643,10 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.0555555555555555</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.444444444444444</c:v>
@@ -2682,10 +2682,10 @@
                   <c:v>0.611111111111111</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.555555555555556</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.222222222222222</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.722222222222222</c:v>
@@ -2760,10 +2760,10 @@
                   <c:v>0.888888888888889</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.611111111111111</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.666666666666667</c:v>
@@ -2799,10 +2799,10 @@
                   <c:v>0.444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.777777777777778</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -2838,10 +2838,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.666666666666667</c:v>
@@ -2856,23 +2856,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="550608696"/>
-        <c:axId val="550605448"/>
+        <c:axId val="526792216"/>
+        <c:axId val="526795464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="550608696"/>
+        <c:axId val="526792216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550605448"/>
+        <c:crossAx val="526795464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="550605448"/>
+        <c:axId val="526795464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2880,7 +2880,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550608696"/>
+        <c:crossAx val="526792216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2947,10 +2947,10 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.0555555555555555</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.444444444444444</c:v>
@@ -2969,11 +2969,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="550593848"/>
-        <c:axId val="550595816"/>
+        <c:axId val="526806344"/>
+        <c:axId val="526822088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="550593848"/>
+        <c:axId val="526806344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2997,14 +2997,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550595816"/>
+        <c:crossAx val="526822088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="550595816"/>
+        <c:axId val="526822088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3030,7 +3030,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550593848"/>
+        <c:crossAx val="526806344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3077,10 +3077,10 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.611111111111111</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.222222222222222</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.888888888888889</c:v>
@@ -3116,10 +3116,10 @@
                   <c:v>0.0555555555555555</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.555555555555556</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.611111111111111</c:v>
@@ -3155,10 +3155,10 @@
                   <c:v>0.555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.222222222222222</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.5</c:v>
@@ -3194,10 +3194,10 @@
                   <c:v>0.444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.722222222222222</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.666666666666667</c:v>
@@ -3233,10 +3233,10 @@
                   <c:v>0.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.388888888888889</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.166666666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.388888888888889</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.777777777777778</c:v>
@@ -3272,10 +3272,10 @@
                   <c:v>0.277777777777778</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.0555555555555555</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.5</c:v>
@@ -3290,23 +3290,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="550532728"/>
-        <c:axId val="550529512"/>
+        <c:axId val="526869512"/>
+        <c:axId val="526872728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="550532728"/>
+        <c:axId val="526869512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550529512"/>
+        <c:crossAx val="526872728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="550529512"/>
+        <c:axId val="526872728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3314,7 +3314,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550532728"/>
+        <c:crossAx val="526869512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3339,9 +3339,7 @@
   <c:lang val="en-US"/>
   <c:style val="18"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3366,10 +3364,10 @@
                   <c:v>0.0555555555555555</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.555555555555556</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.611111111111111</c:v>
@@ -3388,11 +3386,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="550511160"/>
-        <c:axId val="550521320"/>
+        <c:axId val="526886216"/>
+        <c:axId val="526898328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="550511160"/>
+        <c:axId val="526886216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3413,16 +3411,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550521320"/>
+        <c:crossAx val="526898328"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="550521320"/>
+        <c:axId val="526898328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3443,11 +3440,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550511160"/>
+        <c:crossAx val="526886216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3469,9 +3465,7 @@
   <c:lang val="en-US"/>
   <c:style val="18"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3496,10 +3490,10 @@
                   <c:v>0.555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.222222222222222</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.5</c:v>
@@ -3518,11 +3512,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="565571928"/>
-        <c:axId val="565584104"/>
+        <c:axId val="526921736"/>
+        <c:axId val="526919576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565571928"/>
+        <c:axId val="526921736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3543,16 +3537,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565584104"/>
+        <c:crossAx val="526919576"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565584104"/>
+        <c:axId val="526919576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3573,11 +3566,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565571928"/>
+        <c:crossAx val="526921736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3599,9 +3591,7 @@
   <c:lang val="en-US"/>
   <c:style val="18"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3626,10 +3616,10 @@
                   <c:v>0.444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.722222222222222</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.666666666666667</c:v>
@@ -3648,11 +3638,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="565607400"/>
-        <c:axId val="565619576"/>
+        <c:axId val="526957176"/>
+        <c:axId val="526955016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565607400"/>
+        <c:axId val="526957176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3673,16 +3663,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565619576"/>
+        <c:crossAx val="526955016"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565619576"/>
+        <c:axId val="526955016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3703,11 +3692,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565607400"/>
+        <c:crossAx val="526957176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3844,11 +3832,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="551213432"/>
-        <c:axId val="551236104"/>
+        <c:axId val="541792952"/>
+        <c:axId val="541419176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551213432"/>
+        <c:axId val="541792952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3891,13 +3879,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551236104"/>
+        <c:crossAx val="541419176"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551236104"/>
+        <c:axId val="541419176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3921,7 +3909,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551213432"/>
+        <c:crossAx val="541792952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3945,9 +3933,7 @@
   <c:lang val="en-US"/>
   <c:style val="18"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3972,10 +3958,10 @@
                   <c:v>0.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.388888888888889</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.166666666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.388888888888889</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.777777777777778</c:v>
@@ -3994,11 +3980,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="565642888"/>
-        <c:axId val="565655064"/>
+        <c:axId val="526992664"/>
+        <c:axId val="526990504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565642888"/>
+        <c:axId val="526992664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4019,16 +4005,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565655064"/>
+        <c:crossAx val="526990504"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565655064"/>
+        <c:axId val="526990504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4049,11 +4034,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565642888"/>
+        <c:crossAx val="526992664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4100,10 +4084,10 @@
                   <c:v>0.277777777777778</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.0555555555555555</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.5</c:v>
@@ -4122,11 +4106,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="565678440"/>
-        <c:axId val="565690648"/>
+        <c:axId val="527028184"/>
+        <c:axId val="527040392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565678440"/>
+        <c:axId val="527028184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4149,13 +4133,13 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565690648"/>
+        <c:crossAx val="527040392"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565690648"/>
+        <c:axId val="527040392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4179,7 +4163,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565678440"/>
+        <c:crossAx val="527028184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4217,7 +4201,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4265,11 +4248,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="565709736"/>
-        <c:axId val="565722968"/>
+        <c:axId val="527065608"/>
+        <c:axId val="527077032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565709736"/>
+        <c:axId val="527065608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4290,17 +4273,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565722968"/>
+        <c:crossAx val="527077032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565722968"/>
+        <c:axId val="527077032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4322,11 +4304,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565709736"/>
+        <c:crossAx val="527065608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4364,7 +4345,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4390,10 +4370,10 @@
                   <c:v>0.611111111111111</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.555555555555556</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.222222222222222</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.722222222222222</c:v>
@@ -4412,11 +4392,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="565750072"/>
-        <c:axId val="565759304"/>
+        <c:axId val="595194312"/>
+        <c:axId val="657860744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565750072"/>
+        <c:axId val="595194312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4437,17 +4417,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565759304"/>
+        <c:crossAx val="657860744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565759304"/>
+        <c:axId val="657860744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4469,11 +4448,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565750072"/>
+        <c:crossAx val="595194312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4511,7 +4489,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4537,10 +4514,10 @@
                   <c:v>0.888888888888889</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.611111111111111</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.666666666666667</c:v>
@@ -4559,11 +4536,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="565782344"/>
-        <c:axId val="565795624"/>
+        <c:axId val="658062552"/>
+        <c:axId val="658074072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565782344"/>
+        <c:axId val="658062552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4584,17 +4561,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565795624"/>
+        <c:crossAx val="658074072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565795624"/>
+        <c:axId val="658074072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4616,11 +4592,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565782344"/>
+        <c:crossAx val="658062552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4658,7 +4633,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4684,10 +4658,10 @@
                   <c:v>0.444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.777777777777778</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -4706,11 +4680,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="565818952"/>
-        <c:axId val="565832232"/>
+        <c:axId val="658099512"/>
+        <c:axId val="658111048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565818952"/>
+        <c:axId val="658099512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4731,17 +4705,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565832232"/>
+        <c:crossAx val="658111048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565832232"/>
+        <c:axId val="658111048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4763,11 +4736,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565818952"/>
+        <c:crossAx val="658099512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4830,10 +4802,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.666666666666667</c:v>
@@ -4852,11 +4824,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="565855800"/>
-        <c:axId val="565869048"/>
+        <c:axId val="658131032"/>
+        <c:axId val="658144200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565855800"/>
+        <c:axId val="658131032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4879,14 +4851,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565869048"/>
+        <c:crossAx val="658144200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565869048"/>
+        <c:axId val="658144200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4911,7 +4883,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565855800"/>
+        <c:crossAx val="658131032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -5048,11 +5020,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="551259960"/>
-        <c:axId val="551282648"/>
+        <c:axId val="541709208"/>
+        <c:axId val="541665608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551259960"/>
+        <c:axId val="541709208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5095,13 +5067,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551282648"/>
+        <c:crossAx val="541665608"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551282648"/>
+        <c:axId val="541665608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5125,7 +5097,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551259960"/>
+        <c:crossAx val="541709208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5264,11 +5236,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="551308696"/>
-        <c:axId val="551331368"/>
+        <c:axId val="541681384"/>
+        <c:axId val="542063432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551308696"/>
+        <c:axId val="541681384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5311,13 +5283,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551331368"/>
+        <c:crossAx val="542063432"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551331368"/>
+        <c:axId val="542063432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5341,7 +5313,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551308696"/>
+        <c:crossAx val="541681384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5489,11 +5461,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="551370552"/>
-        <c:axId val="551378696"/>
+        <c:axId val="542088248"/>
+        <c:axId val="541355848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551370552"/>
+        <c:axId val="542088248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5536,13 +5508,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551378696"/>
+        <c:crossAx val="541355848"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551378696"/>
+        <c:axId val="541355848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5566,7 +5538,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551370552"/>
+        <c:crossAx val="542088248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5705,11 +5677,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="551402296"/>
-        <c:axId val="551424968"/>
+        <c:axId val="541330488"/>
+        <c:axId val="541309704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551402296"/>
+        <c:axId val="541330488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5752,13 +5724,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551424968"/>
+        <c:crossAx val="541309704"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551424968"/>
+        <c:axId val="541309704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5782,7 +5754,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551402296"/>
+        <c:crossAx val="541330488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5921,11 +5893,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="551455256"/>
-        <c:axId val="551463336"/>
+        <c:axId val="541276168"/>
+        <c:axId val="541270680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551455256"/>
+        <c:axId val="541276168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5959,13 +5931,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551463336"/>
+        <c:crossAx val="541270680"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551463336"/>
+        <c:axId val="541270680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5989,7 +5961,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551455256"/>
+        <c:crossAx val="541276168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6128,11 +6100,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="551496968"/>
-        <c:axId val="551506536"/>
+        <c:axId val="541234408"/>
+        <c:axId val="541227432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551496968"/>
+        <c:axId val="541234408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6175,13 +6147,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551506536"/>
+        <c:crossAx val="541227432"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551506536"/>
+        <c:axId val="541227432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6205,7 +6177,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551496968"/>
+        <c:crossAx val="541234408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6344,11 +6316,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="550868264"/>
-        <c:axId val="550857240"/>
+        <c:axId val="541193576"/>
+        <c:axId val="541186600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="550868264"/>
+        <c:axId val="541193576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6391,13 +6363,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="550857240"/>
+        <c:crossAx val="541186600"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="550857240"/>
+        <c:axId val="541186600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6421,7 +6393,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="550868264"/>
+        <c:crossAx val="541193576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7565,30 +7537,30 @@
     <row r="1" spans="1:8" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1">
       <c r="A1" s="59"/>
       <c r="B1" s="51" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E1" s="58" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="F1" s="58" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G1" s="58" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="H1" s="62" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14" customHeight="1">
-      <c r="A2" s="162" t="s">
-        <v>56</v>
+      <c r="A2" s="165" t="s">
+        <v>65</v>
       </c>
       <c r="B2" s="52">
         <v>1</v>
@@ -7613,7 +7585,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="14" customHeight="1">
-      <c r="A3" s="163"/>
+      <c r="A3" s="166"/>
       <c r="B3" s="53">
         <v>2</v>
       </c>
@@ -7637,7 +7609,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="14" customHeight="1" thickBot="1">
-      <c r="A4" s="164"/>
+      <c r="A4" s="167"/>
       <c r="B4" s="54">
         <v>3</v>
       </c>
@@ -7661,8 +7633,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="14" customHeight="1">
-      <c r="A5" s="165" t="s">
-        <v>43</v>
+      <c r="A5" s="168" t="s">
+        <v>52</v>
       </c>
       <c r="B5" s="55">
         <v>1</v>
@@ -7687,7 +7659,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="14" customHeight="1">
-      <c r="A6" s="165"/>
+      <c r="A6" s="168"/>
       <c r="B6" s="53">
         <v>2</v>
       </c>
@@ -7711,7 +7683,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="14" customHeight="1" thickBot="1">
-      <c r="A7" s="165"/>
+      <c r="A7" s="168"/>
       <c r="B7" s="56">
         <v>3</v>
       </c>
@@ -7735,8 +7707,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="14" customHeight="1">
-      <c r="A8" s="166" t="s">
-        <v>44</v>
+      <c r="A8" s="169" t="s">
+        <v>53</v>
       </c>
       <c r="B8" s="52">
         <v>1</v>
@@ -7761,7 +7733,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="14" customHeight="1">
-      <c r="A9" s="165"/>
+      <c r="A9" s="168"/>
       <c r="B9" s="53">
         <v>2</v>
       </c>
@@ -7785,7 +7757,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="14" customHeight="1" thickBot="1">
-      <c r="A10" s="167"/>
+      <c r="A10" s="170"/>
       <c r="B10" s="54">
         <v>3</v>
       </c>
@@ -7809,8 +7781,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="14" customHeight="1">
-      <c r="A11" s="165" t="s">
-        <v>45</v>
+      <c r="A11" s="168" t="s">
+        <v>54</v>
       </c>
       <c r="B11" s="55">
         <v>2</v>
@@ -7835,7 +7807,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="14" customHeight="1">
-      <c r="A12" s="165"/>
+      <c r="A12" s="168"/>
       <c r="B12" s="53">
         <v>2</v>
       </c>
@@ -7859,7 +7831,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="14" customHeight="1" thickBot="1">
-      <c r="A13" s="165"/>
+      <c r="A13" s="168"/>
       <c r="B13" s="56">
         <v>3</v>
       </c>
@@ -7883,8 +7855,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="14" customHeight="1">
-      <c r="A14" s="166" t="s">
-        <v>46</v>
+      <c r="A14" s="169" t="s">
+        <v>55</v>
       </c>
       <c r="B14" s="52">
         <v>1</v>
@@ -7909,7 +7881,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="14" customHeight="1">
-      <c r="A15" s="165"/>
+      <c r="A15" s="168"/>
       <c r="B15" s="53">
         <v>2</v>
       </c>
@@ -7933,7 +7905,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="14" customHeight="1" thickBot="1">
-      <c r="A16" s="167"/>
+      <c r="A16" s="170"/>
       <c r="B16" s="54">
         <v>3</v>
       </c>
@@ -7957,8 +7929,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="14" customHeight="1">
-      <c r="A17" s="165" t="s">
-        <v>47</v>
+      <c r="A17" s="168" t="s">
+        <v>56</v>
       </c>
       <c r="B17" s="55">
         <v>1</v>
@@ -7983,7 +7955,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="165"/>
+      <c r="A18" s="168"/>
       <c r="B18" s="53">
         <v>2</v>
       </c>
@@ -8007,7 +7979,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="14" thickBot="1">
-      <c r="A19" s="167"/>
+      <c r="A19" s="170"/>
       <c r="B19" s="54">
         <v>3</v>
       </c>
@@ -8034,30 +8006,30 @@
     <row r="21" spans="1:8" ht="14" thickBot="1">
       <c r="A21" s="59"/>
       <c r="B21" s="51" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F21" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="171" t="s">
         <v>66</v>
-      </c>
-      <c r="G21" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" s="61" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="168" t="s">
-        <v>57</v>
       </c>
       <c r="B22" s="52">
         <v>1</v>
@@ -8082,7 +8054,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="169"/>
+      <c r="A23" s="172"/>
       <c r="B23" s="53">
         <v>2</v>
       </c>
@@ -8106,7 +8078,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="14" thickBot="1">
-      <c r="A24" s="170"/>
+      <c r="A24" s="173"/>
       <c r="B24" s="54">
         <v>3</v>
       </c>
@@ -8130,8 +8102,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="160" t="s">
-        <v>58</v>
+      <c r="A25" s="163" t="s">
+        <v>67</v>
       </c>
       <c r="B25" s="55">
         <v>1</v>
@@ -8156,7 +8128,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="160"/>
+      <c r="A26" s="163"/>
       <c r="B26" s="53">
         <v>2</v>
       </c>
@@ -8180,7 +8152,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="14" thickBot="1">
-      <c r="A27" s="160"/>
+      <c r="A27" s="163"/>
       <c r="B27" s="56">
         <v>3</v>
       </c>
@@ -8204,8 +8176,8 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="171" t="s">
-        <v>59</v>
+      <c r="A28" s="174" t="s">
+        <v>68</v>
       </c>
       <c r="B28" s="52">
         <v>1</v>
@@ -8230,7 +8202,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="160"/>
+      <c r="A29" s="163"/>
       <c r="B29" s="53">
         <v>2</v>
       </c>
@@ -8254,7 +8226,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="14" thickBot="1">
-      <c r="A30" s="161"/>
+      <c r="A30" s="164"/>
       <c r="B30" s="54">
         <v>3</v>
       </c>
@@ -8278,8 +8250,8 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="160" t="s">
-        <v>60</v>
+      <c r="A31" s="163" t="s">
+        <v>69</v>
       </c>
       <c r="B31" s="55">
         <v>2</v>
@@ -8304,7 +8276,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="160"/>
+      <c r="A32" s="163"/>
       <c r="B32" s="53">
         <v>2</v>
       </c>
@@ -8328,7 +8300,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="14" thickBot="1">
-      <c r="A33" s="160"/>
+      <c r="A33" s="163"/>
       <c r="B33" s="56">
         <v>3</v>
       </c>
@@ -8352,8 +8324,8 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="171" t="s">
-        <v>61</v>
+      <c r="A34" s="174" t="s">
+        <v>70</v>
       </c>
       <c r="B34" s="52">
         <v>1</v>
@@ -8378,7 +8350,7 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="160"/>
+      <c r="A35" s="163"/>
       <c r="B35" s="53">
         <v>2</v>
       </c>
@@ -8402,7 +8374,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="14" thickBot="1">
-      <c r="A36" s="161"/>
+      <c r="A36" s="164"/>
       <c r="B36" s="54">
         <v>3</v>
       </c>
@@ -8426,8 +8398,8 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="160" t="s">
-        <v>62</v>
+      <c r="A37" s="163" t="s">
+        <v>71</v>
       </c>
       <c r="B37" s="55">
         <v>1</v>
@@ -8452,7 +8424,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="160"/>
+      <c r="A38" s="163"/>
       <c r="B38" s="53">
         <v>2</v>
       </c>
@@ -8476,7 +8448,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="14" thickBot="1">
-      <c r="A39" s="161"/>
+      <c r="A39" s="164"/>
       <c r="B39" s="54">
         <v>3</v>
       </c>
@@ -8500,7 +8472,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="12">
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A2:A4"/>
@@ -8534,8 +8505,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="14"/>
@@ -8550,33 +8521,33 @@
     <row r="1" spans="1:9" ht="29" thickBot="1">
       <c r="A1" s="88"/>
       <c r="B1" s="89" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C1" s="90" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D1" s="91" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E1" s="91" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F1" s="91" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G1" s="91" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H1" s="92" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="I1" s="93" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="13" customHeight="1">
-      <c r="A2" s="180" t="s">
-        <v>79</v>
+      <c r="A2" s="185" t="s">
+        <v>88</v>
       </c>
       <c r="B2" s="95">
         <v>1</v>
@@ -8585,10 +8556,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="97">
+        <v>1</v>
+      </c>
+      <c r="E2" s="97">
         <v>3</v>
-      </c>
-      <c r="E2" s="97">
-        <v>1</v>
       </c>
       <c r="F2" s="97">
         <v>5</v>
@@ -8604,7 +8575,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="13" customHeight="1">
-      <c r="A3" s="181"/>
+      <c r="A3" s="186"/>
       <c r="B3" s="100">
         <v>2</v>
       </c>
@@ -8612,10 +8583,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="102">
+        <v>1</v>
+      </c>
+      <c r="E3" s="102">
         <v>2</v>
-      </c>
-      <c r="E3" s="102">
-        <v>1</v>
       </c>
       <c r="F3" s="102">
         <v>1</v>
@@ -8631,7 +8602,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="13" customHeight="1" thickBot="1">
-      <c r="A4" s="181"/>
+      <c r="A4" s="186"/>
       <c r="B4" s="104">
         <v>3</v>
       </c>
@@ -8639,10 +8610,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="106">
+        <v>4</v>
+      </c>
+      <c r="E4" s="106">
         <v>1</v>
-      </c>
-      <c r="E4" s="106">
-        <v>4</v>
       </c>
       <c r="F4" s="106">
         <v>0</v>
@@ -8660,7 +8631,7 @@
     <row r="5" spans="1:9" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A5" s="108"/>
       <c r="B5" s="109" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C5" s="110">
         <f t="shared" ref="C5:H5" si="0">(weight1*C2+weight2*C3+weight3*C4)/6</f>
@@ -8668,11 +8639,11 @@
       </c>
       <c r="D5" s="110">
         <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E5" s="110">
+        <f>(weight1*E2+weight2*E3+weight3*E4)/6</f>
         <v>1.8333333333333333</v>
-      </c>
-      <c r="E5" s="110">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
       </c>
       <c r="F5" s="110">
         <f t="shared" si="0"/>
@@ -8688,8 +8659,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="13" customHeight="1">
-      <c r="A6" s="180" t="s">
-        <v>81</v>
+      <c r="A6" s="185" t="s">
+        <v>90</v>
       </c>
       <c r="B6" s="112">
         <v>1</v>
@@ -8698,10 +8669,10 @@
         <v>0</v>
       </c>
       <c r="D6" s="114">
+        <v>1</v>
+      </c>
+      <c r="E6" s="114">
         <v>2</v>
-      </c>
-      <c r="E6" s="114">
-        <v>1</v>
       </c>
       <c r="F6" s="114">
         <v>3</v>
@@ -8714,7 +8685,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="13" customHeight="1">
-      <c r="A7" s="181"/>
+      <c r="A7" s="186"/>
       <c r="B7" s="100">
         <v>2</v>
       </c>
@@ -8722,10 +8693,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="102">
+        <v>0</v>
+      </c>
+      <c r="E7" s="102">
         <v>4</v>
-      </c>
-      <c r="E7" s="102">
-        <v>0</v>
       </c>
       <c r="F7" s="102">
         <v>2</v>
@@ -8738,7 +8709,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="13" customHeight="1" thickBot="1">
-      <c r="A8" s="181"/>
+      <c r="A8" s="186"/>
       <c r="B8" s="116">
         <v>3</v>
       </c>
@@ -8746,10 +8717,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="118">
+        <v>5</v>
+      </c>
+      <c r="E8" s="118">
         <v>0</v>
-      </c>
-      <c r="E8" s="118">
-        <v>5</v>
       </c>
       <c r="F8" s="118">
         <v>1</v>
@@ -8764,7 +8735,7 @@
     <row r="9" spans="1:9" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A9" s="108"/>
       <c r="B9" s="109" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C9" s="110">
         <f t="shared" ref="C9:H9" si="1">(weight1*C6+weight2*C7+weight3*C8)/6</f>
@@ -8772,11 +8743,11 @@
       </c>
       <c r="D9" s="110">
         <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="110">
+        <f>(weight1*E6+weight2*E7+weight3*E8)/6</f>
         <v>1.6666666666666667</v>
-      </c>
-      <c r="E9" s="110">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
       </c>
       <c r="F9" s="110">
         <f t="shared" si="1"/>
@@ -8792,8 +8763,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="13" customHeight="1">
-      <c r="A10" s="180" t="s">
-        <v>83</v>
+      <c r="A10" s="185" t="s">
+        <v>0</v>
       </c>
       <c r="B10" s="95">
         <v>1</v>
@@ -8802,10 +8773,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="97">
+        <v>1</v>
+      </c>
+      <c r="E10" s="97">
         <v>0</v>
-      </c>
-      <c r="E10" s="97">
-        <v>1</v>
       </c>
       <c r="F10" s="97">
         <v>2</v>
@@ -8818,7 +8789,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="13" customHeight="1">
-      <c r="A11" s="181"/>
+      <c r="A11" s="186"/>
       <c r="B11" s="100">
         <v>2</v>
       </c>
@@ -8826,10 +8797,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="102">
+        <v>0</v>
+      </c>
+      <c r="E11" s="102">
         <v>4</v>
-      </c>
-      <c r="E11" s="102">
-        <v>0</v>
       </c>
       <c r="F11" s="102">
         <v>3</v>
@@ -8842,7 +8813,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="13" customHeight="1" thickBot="1">
-      <c r="A12" s="181"/>
+      <c r="A12" s="186"/>
       <c r="B12" s="116">
         <v>3</v>
       </c>
@@ -8850,10 +8821,10 @@
         <v>2</v>
       </c>
       <c r="D12" s="118">
+        <v>5</v>
+      </c>
+      <c r="E12" s="118">
         <v>2</v>
-      </c>
-      <c r="E12" s="118">
-        <v>5</v>
       </c>
       <c r="F12" s="118">
         <v>1</v>
@@ -8868,7 +8839,7 @@
     <row r="13" spans="1:9" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A13" s="108"/>
       <c r="B13" s="109" t="s">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="C13" s="110">
         <f t="shared" ref="C13:H13" si="2">(weight1*C10+weight2*C11+weight3*C12)/6</f>
@@ -8876,11 +8847,11 @@
       </c>
       <c r="D13" s="110">
         <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="110">
+        <f>(weight1*E10+weight2*E11+weight3*E12)/6</f>
         <v>0.66666666666666663</v>
-      </c>
-      <c r="E13" s="110">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
       </c>
       <c r="F13" s="110">
         <f t="shared" si="2"/>
@@ -8896,8 +8867,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="13" customHeight="1">
-      <c r="A14" s="180" t="s">
-        <v>85</v>
+      <c r="A14" s="185" t="s">
+        <v>2</v>
       </c>
       <c r="B14" s="112">
         <v>2</v>
@@ -8906,10 +8877,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="114">
+        <v>0</v>
+      </c>
+      <c r="E14" s="114">
         <v>4</v>
-      </c>
-      <c r="E14" s="114">
-        <v>0</v>
       </c>
       <c r="F14" s="114">
         <v>3</v>
@@ -8922,7 +8893,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="13" customHeight="1">
-      <c r="A15" s="181"/>
+      <c r="A15" s="186"/>
       <c r="B15" s="100">
         <v>2</v>
       </c>
@@ -8930,10 +8901,10 @@
         <v>5</v>
       </c>
       <c r="D15" s="102">
+        <v>0</v>
+      </c>
+      <c r="E15" s="102">
         <v>1</v>
-      </c>
-      <c r="E15" s="102">
-        <v>0</v>
       </c>
       <c r="F15" s="102">
         <v>3</v>
@@ -8946,7 +8917,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="13" customHeight="1" thickBot="1">
-      <c r="A16" s="181"/>
+      <c r="A16" s="186"/>
       <c r="B16" s="116">
         <v>3</v>
       </c>
@@ -8954,10 +8925,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="118">
+        <v>6</v>
+      </c>
+      <c r="E16" s="118">
         <v>1</v>
-      </c>
-      <c r="E16" s="118">
-        <v>6</v>
       </c>
       <c r="F16" s="118">
         <v>0</v>
@@ -8972,7 +8943,7 @@
     <row r="17" spans="1:8" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A17" s="108"/>
       <c r="B17" s="109" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="C17" s="110">
         <f t="shared" ref="C17:H17" si="3">(weight1*C14+weight2*C15+weight3*C16)/6</f>
@@ -8980,11 +8951,11 @@
       </c>
       <c r="D17" s="110">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="110">
+        <f>(weight1*E14+weight2*E15+weight3*E16)/6</f>
         <v>2.1666666666666665</v>
-      </c>
-      <c r="E17" s="110">
-        <f t="shared" si="3"/>
-        <v>0</v>
       </c>
       <c r="F17" s="110">
         <f t="shared" si="3"/>
@@ -9000,8 +8971,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="13" customHeight="1">
-      <c r="A18" s="180" t="s">
-        <v>87</v>
+      <c r="A18" s="185" t="s">
+        <v>4</v>
       </c>
       <c r="B18" s="112">
         <v>1</v>
@@ -9026,7 +8997,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="13" customHeight="1">
-      <c r="A19" s="181"/>
+      <c r="A19" s="186"/>
       <c r="B19" s="100">
         <v>2</v>
       </c>
@@ -9034,10 +9005,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="102">
+        <v>4</v>
+      </c>
+      <c r="E19" s="102">
         <v>0</v>
-      </c>
-      <c r="E19" s="102">
-        <v>4</v>
       </c>
       <c r="F19" s="102">
         <v>2</v>
@@ -9050,7 +9021,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="13" customHeight="1" thickBot="1">
-      <c r="A20" s="181"/>
+      <c r="A20" s="186"/>
       <c r="B20" s="116">
         <v>3</v>
       </c>
@@ -9058,10 +9029,10 @@
         <v>2</v>
       </c>
       <c r="D20" s="118">
+        <v>1</v>
+      </c>
+      <c r="E20" s="118">
         <v>5</v>
-      </c>
-      <c r="E20" s="118">
-        <v>1</v>
       </c>
       <c r="F20" s="118">
         <v>0</v>
@@ -9076,7 +9047,7 @@
     <row r="21" spans="1:8" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A21" s="108"/>
       <c r="B21" s="109" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="C21" s="110">
         <f t="shared" ref="C21:H21" si="4">(weight1*C18+weight2*C19+weight3*C20)/6</f>
@@ -9084,11 +9055,11 @@
       </c>
       <c r="D21" s="110">
         <f t="shared" si="4"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="E21" s="110">
+        <f>(weight1*E18+weight2*E19+weight3*E20)/6</f>
         <v>0.5</v>
-      </c>
-      <c r="E21" s="110">
-        <f t="shared" si="4"/>
-        <v>1.1666666666666667</v>
       </c>
       <c r="F21" s="110">
         <f t="shared" si="4"/>
@@ -9104,8 +9075,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="13" customHeight="1">
-      <c r="A22" s="180" t="s">
-        <v>89</v>
+      <c r="A22" s="185" t="s">
+        <v>6</v>
       </c>
       <c r="B22" s="112">
         <v>1</v>
@@ -9114,10 +9085,10 @@
         <v>0</v>
       </c>
       <c r="D22" s="114">
+        <v>3</v>
+      </c>
+      <c r="E22" s="114">
         <v>0</v>
-      </c>
-      <c r="E22" s="114">
-        <v>3</v>
       </c>
       <c r="F22" s="114">
         <v>2</v>
@@ -9130,7 +9101,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="13" customHeight="1">
-      <c r="A23" s="181"/>
+      <c r="A23" s="186"/>
       <c r="B23" s="100">
         <v>2</v>
       </c>
@@ -9138,10 +9109,10 @@
         <v>5</v>
       </c>
       <c r="D23" s="102">
+        <v>0</v>
+      </c>
+      <c r="E23" s="102">
         <v>1</v>
-      </c>
-      <c r="E23" s="102">
-        <v>0</v>
       </c>
       <c r="F23" s="102">
         <v>3</v>
@@ -9154,7 +9125,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="13" customHeight="1" thickBot="1">
-      <c r="A24" s="181"/>
+      <c r="A24" s="186"/>
       <c r="B24" s="116">
         <v>3</v>
       </c>
@@ -9162,10 +9133,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="118">
+        <v>3</v>
+      </c>
+      <c r="E24" s="118">
         <v>5</v>
-      </c>
-      <c r="E24" s="118">
-        <v>3</v>
       </c>
       <c r="F24" s="118">
         <v>1</v>
@@ -9180,7 +9151,7 @@
     <row r="25" spans="1:8" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A25" s="108"/>
       <c r="B25" s="109" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="C25" s="110">
         <f t="shared" ref="C25:H25" si="5">(weight1*C22+weight2*C23+weight3*C24)/6</f>
@@ -9188,11 +9159,11 @@
       </c>
       <c r="D25" s="110">
         <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="E25" s="110">
+        <f>(weight1*E22+weight2*E23+weight3*E24)/6</f>
         <v>0.16666666666666666</v>
-      </c>
-      <c r="E25" s="110">
-        <f t="shared" si="5"/>
-        <v>1.5</v>
       </c>
       <c r="F25" s="110">
         <f t="shared" si="5"/>
@@ -9218,43 +9189,43 @@
       <c r="H26" s="120"/>
     </row>
     <row r="27" spans="1:8" s="125" customFormat="1" ht="29" customHeight="1" thickBot="1">
-      <c r="A27" s="178"/>
-      <c r="B27" s="179"/>
+      <c r="A27" s="183"/>
+      <c r="B27" s="184"/>
       <c r="C27" s="122" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="D27" s="123" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E27" s="123" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F27" s="123" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G27" s="123" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H27" s="124" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A28" s="176" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="177"/>
+      <c r="A28" s="191" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="192"/>
       <c r="C28" s="126">
         <f t="shared" ref="C28:H28" si="6">C5</f>
         <v>1.5</v>
       </c>
       <c r="D28" s="126">
         <f t="shared" si="6"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E28" s="126">
+        <f>E5</f>
         <v>1.8333333333333333</v>
-      </c>
-      <c r="E28" s="126">
-        <f t="shared" si="6"/>
-        <v>0.66666666666666663</v>
       </c>
       <c r="F28" s="126">
         <f t="shared" si="6"/>
@@ -9270,21 +9241,21 @@
       </c>
     </row>
     <row r="29" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A29" s="172" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="173"/>
+      <c r="A29" s="187" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="188"/>
       <c r="C29" s="128">
         <f t="shared" ref="C29:H29" si="7">C9</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="D29" s="128">
         <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="128">
+        <f>E9</f>
         <v>1.6666666666666667</v>
-      </c>
-      <c r="E29" s="128">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
       </c>
       <c r="F29" s="128">
         <f t="shared" si="7"/>
@@ -9300,21 +9271,21 @@
       </c>
     </row>
     <row r="30" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A30" s="172" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="173"/>
+      <c r="A30" s="187" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="188"/>
       <c r="C30" s="128">
         <f t="shared" ref="C30:H30" si="8">C13</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="D30" s="128">
         <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="128">
+        <f>E13</f>
         <v>0.66666666666666663</v>
-      </c>
-      <c r="E30" s="128">
-        <f t="shared" si="8"/>
-        <v>0.5</v>
       </c>
       <c r="F30" s="128">
         <f t="shared" si="8"/>
@@ -9330,21 +9301,21 @@
       </c>
     </row>
     <row r="31" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A31" s="172" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="173"/>
+      <c r="A31" s="187" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="188"/>
       <c r="C31" s="128">
         <f t="shared" ref="C31:H31" si="9">C17</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="D31" s="128">
         <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="128">
+        <f>E17</f>
         <v>2.1666666666666665</v>
-      </c>
-      <c r="E31" s="128">
-        <f t="shared" si="9"/>
-        <v>0</v>
       </c>
       <c r="F31" s="128">
         <f t="shared" si="9"/>
@@ -9360,21 +9331,21 @@
       </c>
     </row>
     <row r="32" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A32" s="172" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="173"/>
+      <c r="A32" s="187" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="188"/>
       <c r="C32" s="128">
         <f t="shared" ref="C32:H32" si="10">C21</f>
         <v>1</v>
       </c>
       <c r="D32" s="128">
         <f t="shared" si="10"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="E32" s="128">
+        <f>E21</f>
         <v>0.5</v>
-      </c>
-      <c r="E32" s="128">
-        <f t="shared" si="10"/>
-        <v>1.1666666666666667</v>
       </c>
       <c r="F32" s="128">
         <f t="shared" si="10"/>
@@ -9390,21 +9361,21 @@
       </c>
     </row>
     <row r="33" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1" thickBot="1">
-      <c r="A33" s="174" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="175"/>
+      <c r="A33" s="189" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="190"/>
       <c r="C33" s="130">
         <f t="shared" ref="C33:H33" si="11">C25</f>
         <v>0.83333333333333337</v>
       </c>
       <c r="D33" s="130">
         <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="E33" s="130">
+        <f>E25</f>
         <v>0.16666666666666666</v>
-      </c>
-      <c r="E33" s="130">
-        <f t="shared" si="11"/>
-        <v>1.5</v>
       </c>
       <c r="F33" s="130">
         <f t="shared" si="11"/>
@@ -9430,46 +9401,46 @@
       <c r="H34" s="120"/>
     </row>
     <row r="35" spans="1:9" s="121" customFormat="1" ht="29" customHeight="1" thickBot="1">
-      <c r="A35" s="178"/>
-      <c r="B35" s="179"/>
+      <c r="A35" s="183"/>
+      <c r="B35" s="184"/>
       <c r="C35" s="122" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D35" s="123" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E35" s="123" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F35" s="123" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G35" s="123" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H35" s="124" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="I35" s="133" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A36" s="176" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="177"/>
+      <c r="A36" s="191" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="192"/>
       <c r="C36" s="126">
         <f t="shared" ref="C36:H36" si="12">(C28-min)/(max-min)</f>
         <v>0.5</v>
       </c>
       <c r="D36" s="126">
         <f t="shared" si="12"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="E36" s="126">
+        <f>(E28-min)/(max-min)</f>
         <v>0.61111111111111105</v>
-      </c>
-      <c r="E36" s="126">
-        <f t="shared" si="12"/>
-        <v>0.22222222222222221</v>
       </c>
       <c r="F36" s="126">
         <f t="shared" si="12"/>
@@ -9488,21 +9459,21 @@
       </c>
     </row>
     <row r="37" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A37" s="172" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="173"/>
+      <c r="A37" s="187" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="188"/>
       <c r="C37" s="126">
         <f t="shared" ref="C37:H37" si="13">(C29-min)/(max-min)</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D37" s="126">
         <f t="shared" si="13"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E37" s="126">
+        <f>(E29-min)/(max-min)</f>
         <v>0.55555555555555558</v>
-      </c>
-      <c r="E37" s="126">
-        <f t="shared" si="13"/>
-        <v>0.16666666666666666</v>
       </c>
       <c r="F37" s="126">
         <f t="shared" si="13"/>
@@ -9521,21 +9492,21 @@
       </c>
     </row>
     <row r="38" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A38" s="172" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="173"/>
+      <c r="A38" s="187" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="188"/>
       <c r="C38" s="126">
         <f t="shared" ref="C38:H38" si="14">(C30-min)/(max-min)</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="D38" s="126">
         <f t="shared" si="14"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E38" s="126">
+        <f>(E30-min)/(max-min)</f>
         <v>0.22222222222222221</v>
-      </c>
-      <c r="E38" s="126">
-        <f t="shared" si="14"/>
-        <v>0.16666666666666666</v>
       </c>
       <c r="F38" s="126">
         <f t="shared" si="14"/>
@@ -9551,21 +9522,21 @@
       </c>
     </row>
     <row r="39" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A39" s="172" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="173"/>
+      <c r="A39" s="187" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="188"/>
       <c r="C39" s="126">
         <f t="shared" ref="C39:H39" si="15">(C31-min)/(max-min)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="D39" s="126">
         <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="126">
+        <f>(E31-min)/(max-min)</f>
         <v>0.72222222222222221</v>
-      </c>
-      <c r="E39" s="126">
-        <f t="shared" si="15"/>
-        <v>0</v>
       </c>
       <c r="F39" s="126">
         <f t="shared" si="15"/>
@@ -9581,21 +9552,21 @@
       </c>
     </row>
     <row r="40" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A40" s="172" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="173"/>
+      <c r="A40" s="187" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="188"/>
       <c r="C40" s="126">
         <f t="shared" ref="C40:H40" si="16">(C32-min)/(max-min)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="D40" s="126">
         <f t="shared" si="16"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E40" s="126">
+        <f>(E32-min)/(max-min)</f>
         <v>0.16666666666666666</v>
-      </c>
-      <c r="E40" s="126">
-        <f t="shared" si="16"/>
-        <v>0.3888888888888889</v>
       </c>
       <c r="F40" s="126">
         <f t="shared" si="16"/>
@@ -9611,21 +9582,21 @@
       </c>
     </row>
     <row r="41" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1" thickBot="1">
-      <c r="A41" s="174" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="175"/>
+      <c r="A41" s="189" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="190"/>
       <c r="C41" s="157">
         <f t="shared" ref="C41:H41" si="17">(C33-min)/(max-min)</f>
         <v>0.27777777777777779</v>
       </c>
       <c r="D41" s="158">
         <f t="shared" si="17"/>
+        <v>0.5</v>
+      </c>
+      <c r="E41" s="158">
+        <f>(E33-min)/(max-min)</f>
         <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E41" s="158">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
       </c>
       <c r="F41" s="158">
         <f t="shared" si="17"/>
@@ -9641,31 +9612,31 @@
       </c>
     </row>
     <row r="42" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1" thickBot="1">
-      <c r="A42" s="188" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="192"/>
-      <c r="C42" s="191">
+      <c r="A42" s="175" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="176"/>
+      <c r="C42" s="162">
         <f>AVERAGE(C36:C41)</f>
         <v>0.3611111111111111</v>
       </c>
-      <c r="D42" s="189">
+      <c r="D42" s="160">
         <f t="shared" ref="D42:H42" si="18">AVERAGE(D36:D41)</f>
+        <v>0.24074074074074073</v>
+      </c>
+      <c r="E42" s="160">
+        <f>AVERAGE(E36:E41)</f>
         <v>0.38888888888888884</v>
       </c>
-      <c r="E42" s="189">
-        <f t="shared" si="18"/>
-        <v>0.24074074074074073</v>
-      </c>
-      <c r="F42" s="189">
+      <c r="F42" s="160">
         <f t="shared" si="18"/>
         <v>0.65740740740740733</v>
       </c>
-      <c r="G42" s="189">
+      <c r="G42" s="160">
         <f t="shared" si="18"/>
         <v>0.44444444444444442</v>
       </c>
-      <c r="H42" s="190">
+      <c r="H42" s="161">
         <f t="shared" si="18"/>
         <v>0.54629629629629628</v>
       </c>
@@ -9675,40 +9646,40 @@
       <c r="A44" s="134"/>
       <c r="B44" s="135"/>
       <c r="C44" s="136" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D44" s="137" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E44" s="137" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F44" s="137" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="G44" s="137" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H44" s="138" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="184" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="185"/>
+      <c r="A45" s="179" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="180"/>
       <c r="C45" s="139">
         <f>C5</f>
         <v>1.5</v>
       </c>
       <c r="D45" s="140">
+        <f>C13</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="E45" s="140">
         <f>C9</f>
         <v>0.16666666666666666</v>
-      </c>
-      <c r="E45" s="140">
-        <f>C13</f>
-        <v>1.6666666666666667</v>
       </c>
       <c r="F45" s="140">
         <f>C17</f>
@@ -9724,81 +9695,81 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="13" customHeight="1">
-      <c r="A46" s="186" t="s">
-        <v>30</v>
-      </c>
-      <c r="B46" s="187"/>
+      <c r="A46" s="181" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="182"/>
       <c r="C46" s="142">
+        <f>E5</f>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="D46" s="143">
+        <f>E13</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E46" s="143">
+        <f>E9</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F46" s="143">
+        <f>E17</f>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="G46" s="143">
+        <f>E21</f>
+        <v>0.5</v>
+      </c>
+      <c r="H46" s="144">
+        <f>E25</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="181" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="182"/>
+      <c r="C47" s="142">
         <f>D5</f>
-        <v>1.8333333333333333</v>
-      </c>
-      <c r="D46" s="143">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D47" s="143">
+        <f>D13</f>
+        <v>0.5</v>
+      </c>
+      <c r="E47" s="143">
         <f>D9</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="E46" s="143">
-        <f>D13</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F46" s="143">
+        <v>0.5</v>
+      </c>
+      <c r="F47" s="143">
         <f>D17</f>
-        <v>2.1666666666666665</v>
-      </c>
-      <c r="G46" s="143">
+        <v>0</v>
+      </c>
+      <c r="G47" s="143">
         <f>D21</f>
-        <v>0.5</v>
-      </c>
-      <c r="H46" s="144">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="H47" s="144">
         <f>D25</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="186" t="s">
-        <v>31</v>
-      </c>
-      <c r="B47" s="187"/>
-      <c r="C47" s="142">
-        <f>E5</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D47" s="143">
-        <f>E9</f>
-        <v>0.5</v>
-      </c>
-      <c r="E47" s="143">
-        <f>E13</f>
-        <v>0.5</v>
-      </c>
-      <c r="F47" s="143">
-        <f>E17</f>
-        <v>0</v>
-      </c>
-      <c r="G47" s="143">
-        <f>E21</f>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="H47" s="144">
-        <f>E25</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="186" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" s="187"/>
+      <c r="A48" s="181" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="182"/>
       <c r="C48" s="142">
         <f>F5</f>
         <v>2.6666666666666665</v>
       </c>
       <c r="D48" s="143">
+        <f>F13</f>
+        <v>1.5</v>
+      </c>
+      <c r="E48" s="143">
         <f>F9</f>
         <v>1.8333333333333333</v>
-      </c>
-      <c r="E48" s="143">
-        <f>F13</f>
-        <v>1.5</v>
       </c>
       <c r="F48" s="143">
         <f>F17</f>
@@ -9814,21 +9785,21 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="186" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" s="187"/>
+      <c r="A49" s="181" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="182"/>
       <c r="C49" s="142">
         <f>G5</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="D49" s="143">
+        <f>G13</f>
+        <v>2</v>
+      </c>
+      <c r="E49" s="143">
         <f>G9</f>
         <v>2.3333333333333335</v>
-      </c>
-      <c r="E49" s="143">
-        <f>G13</f>
-        <v>2</v>
       </c>
       <c r="F49" s="143">
         <f>G17</f>
@@ -9844,21 +9815,21 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1">
-      <c r="A50" s="182" t="s">
-        <v>34</v>
-      </c>
-      <c r="B50" s="183"/>
+      <c r="A50" s="177" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="178"/>
       <c r="C50" s="145">
         <f>H5</f>
         <v>0</v>
       </c>
       <c r="D50" s="146">
+        <f>H13</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="E50" s="146">
         <f>H9</f>
         <v>1.5</v>
-      </c>
-      <c r="E50" s="146">
-        <f>H13</f>
-        <v>1.6666666666666667</v>
       </c>
       <c r="F50" s="146">
         <f>H17</f>
@@ -9875,45 +9846,45 @@
     </row>
     <row r="51" spans="1:8" ht="15" thickBot="1"/>
     <row r="52" spans="1:8" ht="22" customHeight="1" thickBot="1">
-      <c r="A52" s="178" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="179"/>
+      <c r="A52" s="183" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="184"/>
       <c r="C52" s="136" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D52" s="137" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E52" s="137" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F52" s="137" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G52" s="137" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H52" s="138" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="184" t="s">
-        <v>72</v>
-      </c>
-      <c r="B53" s="185"/>
+      <c r="A53" s="179" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="180"/>
       <c r="C53" s="148">
         <f t="shared" ref="C53:H53" si="19">(C45-min)/(max-min)</f>
         <v>0.5</v>
       </c>
       <c r="D53" s="149">
         <f t="shared" si="19"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E53" s="149">
+        <f>(E45-min)/(max-min)</f>
         <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E53" s="149">
-        <f t="shared" si="19"/>
-        <v>0.55555555555555558</v>
       </c>
       <c r="F53" s="149">
         <f t="shared" si="19"/>
@@ -9929,21 +9900,21 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="186" t="s">
-        <v>73</v>
-      </c>
-      <c r="B54" s="187"/>
+      <c r="A54" s="181" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="182"/>
       <c r="C54" s="151">
         <f t="shared" ref="C54:H54" si="20">(C46-min)/(max-min)</f>
         <v>0.61111111111111105</v>
       </c>
       <c r="D54" s="152">
         <f t="shared" si="20"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="E54" s="152">
+        <f>(E46-min)/(max-min)</f>
         <v>0.55555555555555558</v>
-      </c>
-      <c r="E54" s="152">
-        <f t="shared" si="20"/>
-        <v>0.22222222222222221</v>
       </c>
       <c r="F54" s="152">
         <f t="shared" si="20"/>
@@ -9959,10 +9930,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="186" t="s">
-        <v>74</v>
-      </c>
-      <c r="B55" s="187"/>
+      <c r="A55" s="181" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="182"/>
       <c r="C55" s="151">
         <f t="shared" ref="C55:H55" si="21">(C47-min)/(max-min)</f>
         <v>0.22222222222222221</v>
@@ -9972,7 +9943,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E55" s="152">
-        <f t="shared" si="21"/>
+        <f>(E47-min)/(max-min)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="F55" s="152">
@@ -9989,21 +9960,21 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="186" t="s">
-        <v>75</v>
-      </c>
-      <c r="B56" s="187"/>
+      <c r="A56" s="181" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="182"/>
       <c r="C56" s="151">
         <f t="shared" ref="C56:H56" si="22">(C48-min)/(max-min)</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="D56" s="152">
         <f t="shared" si="22"/>
+        <v>0.5</v>
+      </c>
+      <c r="E56" s="152">
+        <f>(E48-min)/(max-min)</f>
         <v>0.61111111111111105</v>
-      </c>
-      <c r="E56" s="152">
-        <f t="shared" si="22"/>
-        <v>0.5</v>
       </c>
       <c r="F56" s="152">
         <f t="shared" si="22"/>
@@ -10019,21 +9990,21 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="186" t="s">
-        <v>76</v>
-      </c>
-      <c r="B57" s="187"/>
+      <c r="A57" s="181" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="182"/>
       <c r="C57" s="151">
         <f t="shared" ref="C57:H57" si="23">(C49-min)/(max-min)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="D57" s="152">
         <f t="shared" si="23"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E57" s="152">
+        <f>(E49-min)/(max-min)</f>
         <v>0.77777777777777779</v>
-      </c>
-      <c r="E57" s="152">
-        <f t="shared" si="23"/>
-        <v>0.66666666666666663</v>
       </c>
       <c r="F57" s="152">
         <f t="shared" si="23"/>
@@ -10049,21 +10020,21 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="15" thickBot="1">
-      <c r="A58" s="182" t="s">
-        <v>77</v>
-      </c>
-      <c r="B58" s="183"/>
+      <c r="A58" s="177" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="178"/>
       <c r="C58" s="154">
         <f t="shared" ref="C58:H58" si="24">(C50-min)/(max-min)</f>
         <v>0</v>
       </c>
       <c r="D58" s="155">
         <f t="shared" si="24"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E58" s="155">
+        <f>(E50-min)/(max-min)</f>
         <v>0.5</v>
-      </c>
-      <c r="E58" s="155">
-        <f t="shared" si="24"/>
-        <v>0.55555555555555558</v>
       </c>
       <c r="F58" s="155">
         <f t="shared" si="24"/>
@@ -10081,6 +10052,26 @@
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="34">
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A45:B45"/>
@@ -10095,29 +10086,9 @@
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C36:H42">
+  <conditionalFormatting sqref="C36:I42">
     <cfRule type="cellIs" dxfId="0" priority="0" stopIfTrue="1" operator="greaterThan">
       <formula>0.6</formula>
     </cfRule>
@@ -10155,30 +10126,30 @@
     <row r="1" spans="1:8" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="11" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B2" s="68"/>
       <c r="C2" s="69"/>
@@ -10190,7 +10161,7 @@
     </row>
     <row r="3" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B3" s="83"/>
       <c r="C3" s="71"/>
@@ -10202,7 +10173,7 @@
     </row>
     <row r="4" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A4" s="6" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B4" s="82"/>
       <c r="C4" s="83"/>
@@ -10214,7 +10185,7 @@
     </row>
     <row r="5" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B5" s="84"/>
       <c r="C5" s="82"/>
@@ -10226,7 +10197,7 @@
     </row>
     <row r="6" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B6" s="79"/>
       <c r="C6" s="81"/>
@@ -10238,7 +10209,7 @@
     </row>
     <row r="7" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A7" s="22" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="80"/>
@@ -10282,30 +10253,30 @@
     <row r="1" spans="1:8" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1">
       <c r="A1" s="3"/>
       <c r="B1" s="11" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="26"/>
@@ -10317,7 +10288,7 @@
     </row>
     <row r="3" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="24"/>
@@ -10329,7 +10300,7 @@
     </row>
     <row r="4" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A4" s="6" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="15"/>
@@ -10341,7 +10312,7 @@
     </row>
     <row r="5" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="2"/>
@@ -10353,7 +10324,7 @@
     </row>
     <row r="6" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="17"/>
@@ -10365,7 +10336,7 @@
     </row>
     <row r="7" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A7" s="22" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="14"/>
@@ -10409,30 +10380,30 @@
     <row r="1" spans="1:8" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1">
       <c r="A1" s="3"/>
       <c r="B1" s="11" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="2"/>
@@ -10444,7 +10415,7 @@
     </row>
     <row r="3" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="17"/>
@@ -10456,7 +10427,7 @@
     </row>
     <row r="4" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="27"/>
@@ -10468,7 +10439,7 @@
     </row>
     <row r="5" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="12"/>
@@ -10480,7 +10451,7 @@
     </row>
     <row r="6" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="24"/>
@@ -10492,7 +10463,7 @@
     </row>
     <row r="7" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A7" s="22" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="19"/>

</xml_diff>

<commit_message>
the field is in the sheep
</commit_message>
<xml_diff>
--- a/earlyUserStudy/earlyStudyResults.xlsx
+++ b/earlyUserStudy/earlyStudyResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29220" yWindow="560" windowWidth="24800" windowHeight="17320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="29220" yWindow="560" windowWidth="24800" windowHeight="17320" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="earlySanalysis" sheetId="3" r:id="rId1"/>
@@ -31,6 +31,42 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+  <si>
+    <t>Window Toggle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active Border</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active Corners</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WEIGHTS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dragging</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rotating</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Resizing</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -363,42 +399,6 @@
     <t>Action Bar</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
-  <si>
-    <t>Window Toggle</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Active Border</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Active Corners</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Other</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>WEIGHTS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dragging</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rotating</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Avg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
@@ -1542,6 +1542,36 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1564,36 +1594,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1739,11 +1739,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541572824"/>
-        <c:axId val="541372984"/>
+        <c:axId val="645300200"/>
+        <c:axId val="645450424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541572824"/>
+        <c:axId val="645300200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,13 +1786,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541372984"/>
+        <c:crossAx val="645450424"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541372984"/>
+        <c:axId val="645450424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,7 +1816,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541572824"/>
+        <c:crossAx val="645300200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1955,11 +1955,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541152312"/>
-        <c:axId val="541145336"/>
+        <c:axId val="608022728"/>
+        <c:axId val="608032280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541152312"/>
+        <c:axId val="608022728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2002,13 +2002,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541145336"/>
+        <c:crossAx val="608032280"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541145336"/>
+        <c:axId val="608032280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2032,7 +2032,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541152312"/>
+        <c:crossAx val="608022728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2171,11 +2171,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541111176"/>
-        <c:axId val="541104200"/>
+        <c:axId val="645628792"/>
+        <c:axId val="645638360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541111176"/>
+        <c:axId val="645628792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2218,13 +2218,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541104200"/>
+        <c:crossAx val="645638360"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541104200"/>
+        <c:axId val="645638360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2248,7 +2248,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541111176"/>
+        <c:crossAx val="645628792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2387,11 +2387,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541069336"/>
-        <c:axId val="526691256"/>
+        <c:axId val="645670664"/>
+        <c:axId val="645680232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541069336"/>
+        <c:axId val="645670664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2434,13 +2434,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526691256"/>
+        <c:crossAx val="645680232"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526691256"/>
+        <c:axId val="645680232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2464,7 +2464,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541069336"/>
+        <c:crossAx val="645670664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2488,9 +2488,7 @@
   <c:lang val="en-US"/>
   <c:style val="18"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2537,11 +2535,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="526731032"/>
-        <c:axId val="526728872"/>
+        <c:axId val="645651512"/>
+        <c:axId val="645430168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="526731032"/>
+        <c:axId val="645651512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2562,16 +2560,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526728872"/>
+        <c:crossAx val="645430168"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526728872"/>
+        <c:axId val="645430168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2592,11 +2589,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526731032"/>
+        <c:crossAx val="645651512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -2856,23 +2852,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="526792216"/>
-        <c:axId val="526795464"/>
+        <c:axId val="608111128"/>
+        <c:axId val="608114408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="526792216"/>
+        <c:axId val="608111128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526795464"/>
+        <c:crossAx val="608114408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="526795464"/>
+        <c:axId val="608114408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2880,7 +2876,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526792216"/>
+        <c:crossAx val="608111128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2921,7 +2917,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2969,11 +2964,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="526806344"/>
-        <c:axId val="526822088"/>
+        <c:axId val="608127944"/>
+        <c:axId val="608137176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="526806344"/>
+        <c:axId val="608127944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2994,17 +2989,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526822088"/>
+        <c:crossAx val="608137176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526822088"/>
+        <c:axId val="608137176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3026,11 +3020,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526806344"/>
+        <c:crossAx val="608127944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3290,23 +3283,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="526869512"/>
-        <c:axId val="526872728"/>
+        <c:axId val="607275256"/>
+        <c:axId val="607272040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="526869512"/>
+        <c:axId val="607275256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526872728"/>
+        <c:crossAx val="607272040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="526872728"/>
+        <c:axId val="607272040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3314,7 +3307,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526869512"/>
+        <c:crossAx val="607275256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3386,11 +3379,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="526886216"/>
-        <c:axId val="526898328"/>
+        <c:axId val="607253688"/>
+        <c:axId val="607263848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="526886216"/>
+        <c:axId val="607253688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3413,13 +3406,13 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526898328"/>
+        <c:crossAx val="607263848"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526898328"/>
+        <c:axId val="607263848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3443,7 +3436,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526886216"/>
+        <c:crossAx val="607253688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3512,11 +3505,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="526921736"/>
-        <c:axId val="526919576"/>
+        <c:axId val="607218104"/>
+        <c:axId val="607228264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="526921736"/>
+        <c:axId val="607218104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3539,13 +3532,13 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526919576"/>
+        <c:crossAx val="607228264"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526919576"/>
+        <c:axId val="607228264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3569,7 +3562,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526921736"/>
+        <c:crossAx val="607218104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3638,11 +3631,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="526957176"/>
-        <c:axId val="526955016"/>
+        <c:axId val="607182632"/>
+        <c:axId val="607192792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="526957176"/>
+        <c:axId val="607182632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3665,13 +3658,13 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526955016"/>
+        <c:crossAx val="607192792"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526955016"/>
+        <c:axId val="607192792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3695,7 +3688,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526957176"/>
+        <c:crossAx val="607182632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3832,11 +3825,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541792952"/>
-        <c:axId val="541419176"/>
+        <c:axId val="645498408"/>
+        <c:axId val="645521112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541792952"/>
+        <c:axId val="645498408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3879,13 +3872,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541419176"/>
+        <c:crossAx val="645521112"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541419176"/>
+        <c:axId val="645521112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3909,7 +3902,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541792952"/>
+        <c:crossAx val="645498408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3980,11 +3973,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="526992664"/>
-        <c:axId val="526990504"/>
+        <c:axId val="607147144"/>
+        <c:axId val="607157256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="526992664"/>
+        <c:axId val="607147144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4007,13 +4000,13 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526990504"/>
+        <c:crossAx val="607157256"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526990504"/>
+        <c:axId val="607157256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4037,7 +4030,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526992664"/>
+        <c:crossAx val="607147144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4106,11 +4099,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="527028184"/>
-        <c:axId val="527040392"/>
+        <c:axId val="652404440"/>
+        <c:axId val="652402296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="527028184"/>
+        <c:axId val="652404440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4133,13 +4126,13 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527040392"/>
+        <c:crossAx val="652402296"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="527040392"/>
+        <c:axId val="652402296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4163,7 +4156,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527028184"/>
+        <c:crossAx val="652404440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4248,11 +4241,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="527065608"/>
-        <c:axId val="527077032"/>
+        <c:axId val="652435688"/>
+        <c:axId val="652448888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="527065608"/>
+        <c:axId val="652435688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4275,14 +4268,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527077032"/>
+        <c:crossAx val="652448888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="527077032"/>
+        <c:axId val="652448888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4307,7 +4300,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527065608"/>
+        <c:crossAx val="652435688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4392,11 +4385,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="595194312"/>
-        <c:axId val="657860744"/>
+        <c:axId val="652476024"/>
+        <c:axId val="652485256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="595194312"/>
+        <c:axId val="652476024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4419,14 +4412,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="657860744"/>
+        <c:crossAx val="652485256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="657860744"/>
+        <c:axId val="652485256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4451,7 +4444,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595194312"/>
+        <c:crossAx val="652476024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4536,11 +4529,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="658062552"/>
-        <c:axId val="658074072"/>
+        <c:axId val="652508296"/>
+        <c:axId val="652521576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="658062552"/>
+        <c:axId val="652508296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4563,14 +4556,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="658074072"/>
+        <c:crossAx val="652521576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="658074072"/>
+        <c:axId val="652521576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4595,7 +4588,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="658062552"/>
+        <c:crossAx val="652508296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4680,11 +4673,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="658099512"/>
-        <c:axId val="658111048"/>
+        <c:axId val="652544904"/>
+        <c:axId val="645661096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="658099512"/>
+        <c:axId val="652544904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4707,14 +4700,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="658111048"/>
+        <c:crossAx val="645661096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="658111048"/>
+        <c:axId val="645661096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4739,7 +4732,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="658099512"/>
+        <c:crossAx val="652544904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4824,11 +4817,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="658131032"/>
-        <c:axId val="658144200"/>
+        <c:axId val="645722904"/>
+        <c:axId val="645736152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="658131032"/>
+        <c:axId val="645722904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4851,14 +4844,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="658144200"/>
+        <c:crossAx val="645736152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="658144200"/>
+        <c:axId val="645736152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4883,7 +4876,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="658131032"/>
+        <c:crossAx val="645722904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -5020,11 +5013,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541709208"/>
-        <c:axId val="541665608"/>
+        <c:axId val="607766600"/>
+        <c:axId val="607789272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541709208"/>
+        <c:axId val="607766600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5067,13 +5060,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541665608"/>
+        <c:crossAx val="607789272"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541665608"/>
+        <c:axId val="607789272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5097,7 +5090,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541709208"/>
+        <c:crossAx val="607766600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5236,11 +5229,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541681384"/>
-        <c:axId val="542063432"/>
+        <c:axId val="607815272"/>
+        <c:axId val="607837944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541681384"/>
+        <c:axId val="607815272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5283,13 +5276,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="542063432"/>
+        <c:crossAx val="607837944"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="542063432"/>
+        <c:axId val="607837944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5313,7 +5306,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541681384"/>
+        <c:crossAx val="607815272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5461,11 +5454,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="542088248"/>
-        <c:axId val="541355848"/>
+        <c:axId val="607877192"/>
+        <c:axId val="607885320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="542088248"/>
+        <c:axId val="607877192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5508,13 +5501,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541355848"/>
+        <c:crossAx val="607885320"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541355848"/>
+        <c:axId val="607885320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5538,7 +5531,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542088248"/>
+        <c:crossAx val="607877192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5677,11 +5670,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541330488"/>
-        <c:axId val="541309704"/>
+        <c:axId val="607908888"/>
+        <c:axId val="607931560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541330488"/>
+        <c:axId val="607908888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5724,13 +5717,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541309704"/>
+        <c:crossAx val="607931560"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541309704"/>
+        <c:axId val="607931560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5754,7 +5747,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541330488"/>
+        <c:crossAx val="607908888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5893,11 +5886,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541276168"/>
-        <c:axId val="541270680"/>
+        <c:axId val="607961832"/>
+        <c:axId val="645494408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541276168"/>
+        <c:axId val="607961832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5931,13 +5924,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541270680"/>
+        <c:crossAx val="645494408"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541270680"/>
+        <c:axId val="645494408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5961,7 +5954,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541276168"/>
+        <c:crossAx val="607961832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6100,11 +6093,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541234408"/>
-        <c:axId val="541227432"/>
+        <c:axId val="645572504"/>
+        <c:axId val="645582072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541234408"/>
+        <c:axId val="645572504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6147,13 +6140,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541227432"/>
+        <c:crossAx val="645582072"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541227432"/>
+        <c:axId val="645582072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6177,7 +6170,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541234408"/>
+        <c:crossAx val="645572504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6316,11 +6309,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="541193576"/>
-        <c:axId val="541186600"/>
+        <c:axId val="607980568"/>
+        <c:axId val="607990136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="541193576"/>
+        <c:axId val="607980568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6363,13 +6356,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541186600"/>
+        <c:crossAx val="607990136"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541186600"/>
+        <c:axId val="607990136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6393,7 +6386,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541193576"/>
+        <c:crossAx val="607980568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7537,30 +7530,30 @@
     <row r="1" spans="1:8" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1">
       <c r="A1" s="59"/>
       <c r="B1" s="51" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E1" s="58" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="F1" s="58" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="G1" s="58" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="H1" s="62" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14" customHeight="1">
       <c r="A2" s="165" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B2" s="52">
         <v>1</v>
@@ -7634,7 +7627,7 @@
     </row>
     <row r="5" spans="1:8" ht="14" customHeight="1">
       <c r="A5" s="168" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B5" s="55">
         <v>1</v>
@@ -7708,7 +7701,7 @@
     </row>
     <row r="8" spans="1:8" ht="14" customHeight="1">
       <c r="A8" s="169" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B8" s="52">
         <v>1</v>
@@ -7782,7 +7775,7 @@
     </row>
     <row r="11" spans="1:8" ht="14" customHeight="1">
       <c r="A11" s="168" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B11" s="55">
         <v>2</v>
@@ -7856,7 +7849,7 @@
     </row>
     <row r="14" spans="1:8" ht="14" customHeight="1">
       <c r="A14" s="169" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B14" s="52">
         <v>1</v>
@@ -7930,7 +7923,7 @@
     </row>
     <row r="17" spans="1:8" ht="14" customHeight="1">
       <c r="A17" s="168" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B17" s="55">
         <v>1</v>
@@ -8006,30 +7999,30 @@
     <row r="21" spans="1:8" ht="14" thickBot="1">
       <c r="A21" s="59"/>
       <c r="B21" s="51" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="F21" s="61" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G21" s="61" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H21" s="61" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="171" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B22" s="52">
         <v>1</v>
@@ -8103,7 +8096,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="163" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B25" s="55">
         <v>1</v>
@@ -8177,7 +8170,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="174" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B28" s="52">
         <v>1</v>
@@ -8251,7 +8244,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="163" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B31" s="55">
         <v>2</v>
@@ -8325,7 +8318,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="174" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B34" s="52">
         <v>1</v>
@@ -8399,7 +8392,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="163" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B37" s="55">
         <v>1</v>
@@ -8505,7 +8498,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:H42"/>
     </sheetView>
   </sheetViews>
@@ -8521,33 +8514,33 @@
     <row r="1" spans="1:9" ht="29" thickBot="1">
       <c r="A1" s="88"/>
       <c r="B1" s="89" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C1" s="90" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D1" s="91" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="E1" s="91" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F1" s="91" t="s">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="G1" s="91" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="H1" s="92" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="I1" s="93" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="13" customHeight="1">
-      <c r="A2" s="185" t="s">
-        <v>88</v>
+      <c r="A2" s="183" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="95">
         <v>1</v>
@@ -8575,7 +8568,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="13" customHeight="1">
-      <c r="A3" s="186"/>
+      <c r="A3" s="184"/>
       <c r="B3" s="100">
         <v>2</v>
       </c>
@@ -8602,7 +8595,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="13" customHeight="1" thickBot="1">
-      <c r="A4" s="186"/>
+      <c r="A4" s="184"/>
       <c r="B4" s="104">
         <v>3</v>
       </c>
@@ -8631,7 +8624,7 @@
     <row r="5" spans="1:9" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A5" s="108"/>
       <c r="B5" s="109" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="C5" s="110">
         <f t="shared" ref="C5:H5" si="0">(weight1*C2+weight2*C3+weight3*C4)/6</f>
@@ -8659,8 +8652,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="13" customHeight="1">
-      <c r="A6" s="185" t="s">
-        <v>90</v>
+      <c r="A6" s="183" t="s">
+        <v>7</v>
       </c>
       <c r="B6" s="112">
         <v>1</v>
@@ -8685,7 +8678,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="13" customHeight="1">
-      <c r="A7" s="186"/>
+      <c r="A7" s="184"/>
       <c r="B7" s="100">
         <v>2</v>
       </c>
@@ -8709,7 +8702,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="13" customHeight="1" thickBot="1">
-      <c r="A8" s="186"/>
+      <c r="A8" s="184"/>
       <c r="B8" s="116">
         <v>3</v>
       </c>
@@ -8735,7 +8728,7 @@
     <row r="9" spans="1:9" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A9" s="108"/>
       <c r="B9" s="109" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C9" s="110">
         <f t="shared" ref="C9:H9" si="1">(weight1*C6+weight2*C7+weight3*C8)/6</f>
@@ -8763,8 +8756,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="13" customHeight="1">
-      <c r="A10" s="185" t="s">
-        <v>0</v>
+      <c r="A10" s="183" t="s">
+        <v>9</v>
       </c>
       <c r="B10" s="95">
         <v>1</v>
@@ -8789,7 +8782,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="13" customHeight="1">
-      <c r="A11" s="186"/>
+      <c r="A11" s="184"/>
       <c r="B11" s="100">
         <v>2</v>
       </c>
@@ -8813,7 +8806,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="13" customHeight="1" thickBot="1">
-      <c r="A12" s="186"/>
+      <c r="A12" s="184"/>
       <c r="B12" s="116">
         <v>3</v>
       </c>
@@ -8839,7 +8832,7 @@
     <row r="13" spans="1:9" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A13" s="108"/>
       <c r="B13" s="109" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C13" s="110">
         <f t="shared" ref="C13:H13" si="2">(weight1*C10+weight2*C11+weight3*C12)/6</f>
@@ -8867,8 +8860,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="13" customHeight="1">
-      <c r="A14" s="185" t="s">
-        <v>2</v>
+      <c r="A14" s="183" t="s">
+        <v>11</v>
       </c>
       <c r="B14" s="112">
         <v>2</v>
@@ -8893,7 +8886,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="13" customHeight="1">
-      <c r="A15" s="186"/>
+      <c r="A15" s="184"/>
       <c r="B15" s="100">
         <v>2</v>
       </c>
@@ -8917,7 +8910,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="13" customHeight="1" thickBot="1">
-      <c r="A16" s="186"/>
+      <c r="A16" s="184"/>
       <c r="B16" s="116">
         <v>3</v>
       </c>
@@ -8943,7 +8936,7 @@
     <row r="17" spans="1:8" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A17" s="108"/>
       <c r="B17" s="109" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C17" s="110">
         <f t="shared" ref="C17:H17" si="3">(weight1*C14+weight2*C15+weight3*C16)/6</f>
@@ -8971,8 +8964,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="13" customHeight="1">
-      <c r="A18" s="185" t="s">
-        <v>4</v>
+      <c r="A18" s="183" t="s">
+        <v>13</v>
       </c>
       <c r="B18" s="112">
         <v>1</v>
@@ -8997,7 +8990,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="13" customHeight="1">
-      <c r="A19" s="186"/>
+      <c r="A19" s="184"/>
       <c r="B19" s="100">
         <v>2</v>
       </c>
@@ -9021,7 +9014,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="13" customHeight="1" thickBot="1">
-      <c r="A20" s="186"/>
+      <c r="A20" s="184"/>
       <c r="B20" s="116">
         <v>3</v>
       </c>
@@ -9047,7 +9040,7 @@
     <row r="21" spans="1:8" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A21" s="108"/>
       <c r="B21" s="109" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C21" s="110">
         <f t="shared" ref="C21:H21" si="4">(weight1*C18+weight2*C19+weight3*C20)/6</f>
@@ -9075,8 +9068,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="13" customHeight="1">
-      <c r="A22" s="185" t="s">
-        <v>6</v>
+      <c r="A22" s="183" t="s">
+        <v>15</v>
       </c>
       <c r="B22" s="112">
         <v>1</v>
@@ -9101,7 +9094,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="13" customHeight="1">
-      <c r="A23" s="186"/>
+      <c r="A23" s="184"/>
       <c r="B23" s="100">
         <v>2</v>
       </c>
@@ -9125,7 +9118,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="13" customHeight="1" thickBot="1">
-      <c r="A24" s="186"/>
+      <c r="A24" s="184"/>
       <c r="B24" s="116">
         <v>3</v>
       </c>
@@ -9151,7 +9144,7 @@
     <row r="25" spans="1:8" s="111" customFormat="1" ht="13" customHeight="1" thickBot="1">
       <c r="A25" s="108"/>
       <c r="B25" s="109" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C25" s="110">
         <f t="shared" ref="C25:H25" si="5">(weight1*C22+weight2*C23+weight3*C24)/6</f>
@@ -9189,32 +9182,32 @@
       <c r="H26" s="120"/>
     </row>
     <row r="27" spans="1:8" s="125" customFormat="1" ht="29" customHeight="1" thickBot="1">
-      <c r="A27" s="183"/>
-      <c r="B27" s="184"/>
+      <c r="A27" s="181"/>
+      <c r="B27" s="182"/>
       <c r="C27" s="122" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D27" s="123" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E27" s="123" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F27" s="123" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G27" s="123" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H27" s="124" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A28" s="191" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="192"/>
+      <c r="A28" s="179" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="180"/>
       <c r="C28" s="126">
         <f t="shared" ref="C28:H28" si="6">C5</f>
         <v>1.5</v>
@@ -9241,10 +9234,10 @@
       </c>
     </row>
     <row r="29" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A29" s="187" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="188"/>
+      <c r="A29" s="175" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="176"/>
       <c r="C29" s="128">
         <f t="shared" ref="C29:H29" si="7">C9</f>
         <v>0.16666666666666666</v>
@@ -9271,10 +9264,10 @@
       </c>
     </row>
     <row r="30" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A30" s="187" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="188"/>
+      <c r="A30" s="175" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="176"/>
       <c r="C30" s="128">
         <f t="shared" ref="C30:H30" si="8">C13</f>
         <v>1.6666666666666667</v>
@@ -9301,10 +9294,10 @@
       </c>
     </row>
     <row r="31" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A31" s="187" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="188"/>
+      <c r="A31" s="175" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="176"/>
       <c r="C31" s="128">
         <f t="shared" ref="C31:H31" si="9">C17</f>
         <v>1.3333333333333333</v>
@@ -9331,10 +9324,10 @@
       </c>
     </row>
     <row r="32" spans="1:8" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A32" s="187" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="188"/>
+      <c r="A32" s="175" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="176"/>
       <c r="C32" s="128">
         <f t="shared" ref="C32:H32" si="10">C21</f>
         <v>1</v>
@@ -9361,10 +9354,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1" thickBot="1">
-      <c r="A33" s="189" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="190"/>
+      <c r="A33" s="177" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="178"/>
       <c r="C33" s="130">
         <f t="shared" ref="C33:H33" si="11">C25</f>
         <v>0.83333333333333337</v>
@@ -9401,35 +9394,35 @@
       <c r="H34" s="120"/>
     </row>
     <row r="35" spans="1:9" s="121" customFormat="1" ht="29" customHeight="1" thickBot="1">
-      <c r="A35" s="183"/>
-      <c r="B35" s="184"/>
+      <c r="A35" s="181"/>
+      <c r="B35" s="182"/>
       <c r="C35" s="122" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D35" s="123" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E35" s="123" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F35" s="123" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="G35" s="123" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H35" s="124" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="I35" s="133" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A36" s="191" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="192"/>
+      <c r="A36" s="179" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="180"/>
       <c r="C36" s="126">
         <f t="shared" ref="C36:H36" si="12">(C28-min)/(max-min)</f>
         <v>0.5</v>
@@ -9439,7 +9432,7 @@
         <v>0.22222222222222221</v>
       </c>
       <c r="E36" s="126">
-        <f>(E28-min)/(max-min)</f>
+        <f t="shared" ref="E36:E41" si="13">(E28-min)/(max-min)</f>
         <v>0.61111111111111105</v>
       </c>
       <c r="F36" s="126">
@@ -9459,169 +9452,169 @@
       </c>
     </row>
     <row r="37" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A37" s="187" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="188"/>
+      <c r="A37" s="175" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="176"/>
       <c r="C37" s="126">
-        <f t="shared" ref="C37:H37" si="13">(C29-min)/(max-min)</f>
+        <f t="shared" ref="C37:H37" si="14">(C29-min)/(max-min)</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D37" s="126">
+        <f t="shared" si="14"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E37" s="126">
+        <f t="shared" si="13"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="F37" s="126">
+        <f t="shared" si="14"/>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="G37" s="126">
+        <f t="shared" si="14"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="H37" s="127">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="I37" s="133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
+      <c r="A38" s="175" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="176"/>
+      <c r="C38" s="126">
+        <f t="shared" ref="C38:H38" si="15">(C30-min)/(max-min)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D38" s="126">
+        <f t="shared" si="15"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E38" s="126">
+        <f t="shared" si="13"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="F38" s="126">
+        <f t="shared" si="15"/>
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="126">
+        <f t="shared" si="15"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H38" s="127">
+        <f t="shared" si="15"/>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
+      <c r="A39" s="175" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="176"/>
+      <c r="C39" s="126">
+        <f t="shared" ref="C39:H39" si="16">(C31-min)/(max-min)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D39" s="126">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="126">
+        <f t="shared" si="13"/>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="F39" s="126">
+        <f t="shared" si="16"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G39" s="126">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="127">
+        <f t="shared" si="16"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
+      <c r="A40" s="175" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="176"/>
+      <c r="C40" s="126">
+        <f t="shared" ref="C40:H40" si="17">(C32-min)/(max-min)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D40" s="126">
+        <f t="shared" si="17"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E40" s="126">
         <f t="shared" si="13"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E37" s="126">
-        <f>(E29-min)/(max-min)</f>
+      <c r="F40" s="126">
+        <f t="shared" si="17"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="G40" s="126">
+        <f t="shared" si="17"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H40" s="127">
+        <f t="shared" si="17"/>
         <v>0.55555555555555558</v>
       </c>
-      <c r="F37" s="126">
+    </row>
+    <row r="41" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1" thickBot="1">
+      <c r="A41" s="177" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="178"/>
+      <c r="C41" s="157">
+        <f t="shared" ref="C41:H41" si="18">(C33-min)/(max-min)</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D41" s="158">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="E41" s="158">
         <f t="shared" si="13"/>
-        <v>0.61111111111111105</v>
-      </c>
-      <c r="G37" s="126">
-        <f t="shared" si="13"/>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="H37" s="127">
-        <f t="shared" si="13"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="F41" s="158">
+        <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
-      <c r="I37" s="133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A38" s="187" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="188"/>
-      <c r="C38" s="126">
-        <f t="shared" ref="C38:H38" si="14">(C30-min)/(max-min)</f>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="D38" s="126">
-        <f t="shared" si="14"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="E38" s="126">
-        <f>(E30-min)/(max-min)</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="F38" s="126">
-        <f t="shared" si="14"/>
-        <v>0.5</v>
-      </c>
-      <c r="G38" s="126">
-        <f t="shared" si="14"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="H38" s="127">
-        <f t="shared" si="14"/>
-        <v>0.55555555555555558</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A39" s="187" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="188"/>
-      <c r="C39" s="126">
-        <f t="shared" ref="C39:H39" si="15">(C31-min)/(max-min)</f>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="D39" s="126">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="126">
-        <f>(E31-min)/(max-min)</f>
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="F39" s="126">
-        <f t="shared" si="15"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G39" s="126">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H39" s="127">
-        <f t="shared" si="15"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1">
-      <c r="A40" s="187" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="188"/>
-      <c r="C40" s="126">
-        <f t="shared" ref="C40:H40" si="16">(C32-min)/(max-min)</f>
+      <c r="G41" s="158">
+        <f t="shared" si="18"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D40" s="126">
-        <f t="shared" si="16"/>
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="E40" s="126">
-        <f>(E32-min)/(max-min)</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F40" s="126">
-        <f t="shared" si="16"/>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="G40" s="126">
-        <f t="shared" si="16"/>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="H40" s="127">
-        <f t="shared" si="16"/>
-        <v>0.55555555555555558</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1" thickBot="1">
-      <c r="A41" s="189" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="190"/>
-      <c r="C41" s="157">
-        <f t="shared" ref="C41:H41" si="17">(C33-min)/(max-min)</f>
-        <v>0.27777777777777779</v>
-      </c>
-      <c r="D41" s="158">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="E41" s="158">
-        <f>(E33-min)/(max-min)</f>
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="F41" s="158">
-        <f t="shared" si="17"/>
-        <v>0.5</v>
-      </c>
-      <c r="G41" s="158">
-        <f t="shared" si="17"/>
-        <v>0.33333333333333331</v>
-      </c>
       <c r="H41" s="131">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="121" customFormat="1" ht="13" customHeight="1" thickBot="1">
-      <c r="A42" s="175" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="176"/>
+      <c r="A42" s="185" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="186"/>
       <c r="C42" s="162">
         <f>AVERAGE(C36:C41)</f>
         <v>0.3611111111111111</v>
       </c>
       <c r="D42" s="160">
-        <f t="shared" ref="D42:H42" si="18">AVERAGE(D36:D41)</f>
+        <f t="shared" ref="D42:H42" si="19">AVERAGE(D36:D41)</f>
         <v>0.24074074074074073</v>
       </c>
       <c r="E42" s="160">
@@ -9629,15 +9622,15 @@
         <v>0.38888888888888884</v>
       </c>
       <c r="F42" s="160">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.65740740740740733</v>
       </c>
       <c r="G42" s="160">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="H42" s="161">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.54629629629629628</v>
       </c>
     </row>
@@ -9646,29 +9639,29 @@
       <c r="A44" s="134"/>
       <c r="B44" s="135"/>
       <c r="C44" s="136" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D44" s="137" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E44" s="137" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F44" s="137" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G44" s="137" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H44" s="138" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="179" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="180"/>
+      <c r="A45" s="189" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="190"/>
       <c r="C45" s="139">
         <f>C5</f>
         <v>1.5</v>
@@ -9695,10 +9688,10 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="13" customHeight="1">
-      <c r="A46" s="181" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="182"/>
+      <c r="A46" s="191" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="192"/>
       <c r="C46" s="142">
         <f>E5</f>
         <v>1.8333333333333333</v>
@@ -9725,10 +9718,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="181" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="182"/>
+      <c r="A47" s="191" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="192"/>
       <c r="C47" s="142">
         <f>D5</f>
         <v>0.66666666666666663</v>
@@ -9755,10 +9748,10 @@
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="181" t="s">
-        <v>41</v>
-      </c>
-      <c r="B48" s="182"/>
+      <c r="A48" s="191" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="192"/>
       <c r="C48" s="142">
         <f>F5</f>
         <v>2.6666666666666665</v>
@@ -9785,10 +9778,10 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="181" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="182"/>
+      <c r="A49" s="191" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="192"/>
       <c r="C49" s="142">
         <f>G5</f>
         <v>1.3333333333333333</v>
@@ -9815,10 +9808,10 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1">
-      <c r="A50" s="177" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="178"/>
+      <c r="A50" s="187" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="188"/>
       <c r="C50" s="145">
         <f>H5</f>
         <v>0</v>
@@ -9846,232 +9839,211 @@
     </row>
     <row r="51" spans="1:8" ht="15" thickBot="1"/>
     <row r="52" spans="1:8" ht="22" customHeight="1" thickBot="1">
-      <c r="A52" s="183" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" s="184"/>
+      <c r="A52" s="181" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="182"/>
       <c r="C52" s="136" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D52" s="137" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E52" s="137" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F52" s="137" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G52" s="137" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H52" s="138" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="179" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" s="180"/>
+      <c r="A53" s="189" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="190"/>
       <c r="C53" s="148">
-        <f t="shared" ref="C53:H53" si="19">(C45-min)/(max-min)</f>
+        <f t="shared" ref="C53:H53" si="20">(C45-min)/(max-min)</f>
         <v>0.5</v>
       </c>
       <c r="D53" s="149">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="E53" s="149">
-        <f>(E45-min)/(max-min)</f>
+        <f t="shared" ref="E53:E58" si="21">(E45-min)/(max-min)</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="F53" s="149">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="G53" s="149">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H53" s="150">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.27777777777777779</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="181" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" s="182"/>
+      <c r="A54" s="191" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="192"/>
       <c r="C54" s="151">
-        <f t="shared" ref="C54:H54" si="20">(C46-min)/(max-min)</f>
+        <f t="shared" ref="C54:H54" si="22">(C46-min)/(max-min)</f>
         <v>0.61111111111111105</v>
       </c>
       <c r="D54" s="152">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="E54" s="152">
-        <f>(E46-min)/(max-min)</f>
+        <f t="shared" si="21"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="F54" s="152">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.72222222222222221</v>
       </c>
       <c r="G54" s="152">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H54" s="153">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="181" t="s">
-        <v>83</v>
-      </c>
-      <c r="B55" s="182"/>
+      <c r="A55" s="191" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="192"/>
       <c r="C55" s="151">
-        <f t="shared" ref="C55:H55" si="21">(C47-min)/(max-min)</f>
+        <f t="shared" ref="C55:H55" si="23">(C47-min)/(max-min)</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="D55" s="152">
+        <f t="shared" si="23"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E55" s="152">
         <f t="shared" si="21"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E55" s="152">
-        <f>(E47-min)/(max-min)</f>
-        <v>0.16666666666666666</v>
-      </c>
       <c r="F55" s="152">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="G55" s="152">
+        <f t="shared" si="23"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="H55" s="153">
+        <f t="shared" si="23"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="191" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="192"/>
+      <c r="C56" s="151">
+        <f t="shared" ref="C56:H56" si="24">(C48-min)/(max-min)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D56" s="152">
+        <f t="shared" si="24"/>
+        <v>0.5</v>
+      </c>
+      <c r="E56" s="152">
         <f t="shared" si="21"/>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="F56" s="152">
+        <f t="shared" si="24"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G56" s="152">
+        <f t="shared" si="24"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="H56" s="153">
+        <f t="shared" si="24"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="192"/>
+      <c r="C57" s="151">
+        <f t="shared" ref="C57:H57" si="25">(C49-min)/(max-min)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D57" s="152">
+        <f t="shared" si="25"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E57" s="152">
+        <f t="shared" si="21"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="F57" s="152">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="G55" s="152">
-        <f t="shared" si="21"/>
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="H55" s="153">
+      <c r="G57" s="152">
+        <f t="shared" si="25"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H57" s="153">
+        <f t="shared" si="25"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" thickBot="1">
+      <c r="A58" s="187" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="188"/>
+      <c r="C58" s="154">
+        <f t="shared" ref="C58:H58" si="26">(C50-min)/(max-min)</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="155">
+        <f t="shared" si="26"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E58" s="155">
         <f t="shared" si="21"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="181" t="s">
-        <v>84</v>
-      </c>
-      <c r="B56" s="182"/>
-      <c r="C56" s="151">
-        <f t="shared" ref="C56:H56" si="22">(C48-min)/(max-min)</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="D56" s="152">
-        <f t="shared" si="22"/>
-        <v>0.5</v>
-      </c>
-      <c r="E56" s="152">
-        <f>(E48-min)/(max-min)</f>
-        <v>0.61111111111111105</v>
-      </c>
-      <c r="F56" s="152">
-        <f t="shared" si="22"/>
+      <c r="F58" s="155">
+        <f t="shared" si="26"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G56" s="152">
-        <f t="shared" si="22"/>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="H56" s="153">
-        <f t="shared" si="22"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="181" t="s">
-        <v>85</v>
-      </c>
-      <c r="B57" s="182"/>
-      <c r="C57" s="151">
-        <f t="shared" ref="C57:H57" si="23">(C49-min)/(max-min)</f>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="D57" s="152">
-        <f t="shared" si="23"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E57" s="152">
-        <f>(E49-min)/(max-min)</f>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="F57" s="152">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="G57" s="152">
-        <f t="shared" si="23"/>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="H57" s="153">
-        <f t="shared" si="23"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="15" thickBot="1">
-      <c r="A58" s="177" t="s">
-        <v>86</v>
-      </c>
-      <c r="B58" s="178"/>
-      <c r="C58" s="154">
-        <f t="shared" ref="C58:H58" si="24">(C50-min)/(max-min)</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="155">
-        <f t="shared" si="24"/>
+      <c r="G58" s="155">
+        <f t="shared" si="26"/>
         <v>0.55555555555555558</v>
       </c>
-      <c r="E58" s="155">
-        <f>(E50-min)/(max-min)</f>
-        <v>0.5</v>
-      </c>
-      <c r="F58" s="155">
-        <f t="shared" si="24"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G58" s="155">
-        <f t="shared" si="24"/>
-        <v>0.55555555555555558</v>
-      </c>
       <c r="H58" s="156">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="34">
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A20"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A45:B45"/>
@@ -10086,6 +10058,26 @@
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C36:I42">
@@ -10094,7 +10086,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75196850393700787" right="0.75196850393700787" top="0.56666666666666665" bottom="0.7" header="0.35555555555555557" footer="0.41111111111111109"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;Cresult analysis average</oddHeader>
   </headerFooter>
@@ -10126,30 +10117,30 @@
     <row r="1" spans="1:8" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="11" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B2" s="68"/>
       <c r="C2" s="69"/>
@@ -10161,7 +10152,7 @@
     </row>
     <row r="3" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B3" s="83"/>
       <c r="C3" s="71"/>
@@ -10173,7 +10164,7 @@
     </row>
     <row r="4" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A4" s="6" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B4" s="82"/>
       <c r="C4" s="83"/>
@@ -10185,7 +10176,7 @@
     </row>
     <row r="5" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A5" s="6" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B5" s="84"/>
       <c r="C5" s="82"/>
@@ -10197,7 +10188,7 @@
     </row>
     <row r="6" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B6" s="79"/>
       <c r="C6" s="81"/>
@@ -10209,7 +10200,7 @@
     </row>
     <row r="7" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A7" s="22" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="80"/>
@@ -10220,7 +10211,6 @@
       <c r="H7" s="20"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75196850393700787" right="0.75196850393700787" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -10240,8 +10230,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -10253,30 +10243,30 @@
     <row r="1" spans="1:8" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1">
       <c r="A1" s="3"/>
       <c r="B1" s="11" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="26"/>
@@ -10288,7 +10278,7 @@
     </row>
     <row r="3" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="24"/>
@@ -10300,7 +10290,7 @@
     </row>
     <row r="4" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A4" s="6" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="15"/>
@@ -10312,7 +10302,7 @@
     </row>
     <row r="5" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A5" s="6" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="2"/>
@@ -10324,7 +10314,7 @@
     </row>
     <row r="6" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="17"/>
@@ -10336,7 +10326,7 @@
     </row>
     <row r="7" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A7" s="22" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="14"/>
@@ -10347,12 +10337,11 @@
       <c r="H7" s="20"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;14TIDE Early Usability Study (1)</oddHeader>
+    <oddHeader>&amp;C&amp;14TIDE Design Experiment (1)</oddHeader>
   </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -10380,30 +10369,30 @@
     <row r="1" spans="1:8" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1">
       <c r="A1" s="3"/>
       <c r="B1" s="11" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="2"/>
@@ -10415,7 +10404,7 @@
     </row>
     <row r="3" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="17"/>
@@ -10427,7 +10416,7 @@
     </row>
     <row r="4" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="27"/>
@@ -10439,7 +10428,7 @@
     </row>
     <row r="5" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="12"/>
@@ -10451,7 +10440,7 @@
     </row>
     <row r="6" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="24"/>
@@ -10463,7 +10452,7 @@
     </row>
     <row r="7" spans="1:8" ht="43" customHeight="1" thickBot="1">
       <c r="A7" s="22" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="19"/>
@@ -10474,7 +10463,6 @@
       <c r="H7" s="20"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>